<commit_message>
Angle of rotation files updates
</commit_message>
<xml_diff>
--- a/quantifyVagusNerve/Data/Supporting Files/Angle of Rotation/Angle_of_rotation_Barycenter_complete_1_0.1.xlsx
+++ b/quantifyVagusNerve/Data/Supporting Files/Angle of Rotation/Angle_of_rotation_Barycenter_complete_1_0.1.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanja\Documents\GitHub\spatial-neuro\quantifyVagusNerve\Data\Supporting Files\Angle of Rotation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6BBFE9-D981-4949-AD4F-7B7356E90558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE5C2F0-953C-4187-8807-741ABB206B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Min angle matrix" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -24,7 +29,7 @@
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -80,41 +85,45 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -143,9 +152,13 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -183,166 +196,142 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
@@ -350,99 +339,99 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:AC29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>0</v>
       </c>
       <c r="B1">
-        <v>315</v>
+        <v>270</v>
       </c>
       <c r="C1">
-        <v>0</v>
+        <v>315</v>
       </c>
       <c r="D1">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="E1">
         <v>270</v>
       </c>
       <c r="F1">
-        <v>135</v>
+        <v>0</v>
       </c>
       <c r="G1">
-        <v>135</v>
+        <v>45</v>
       </c>
       <c r="H1">
-        <v>315</v>
+        <v>270</v>
       </c>
       <c r="I1">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="J1">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="K1">
         <v>225</v>
       </c>
       <c r="L1">
-        <v>180</v>
+        <v>225</v>
       </c>
       <c r="M1">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="N1">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="O1">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="P1">
-        <v>315</v>
+        <v>270</v>
       </c>
       <c r="Q1">
-        <v>135</v>
+        <v>45</v>
       </c>
       <c r="R1">
-        <v>135</v>
+        <v>45</v>
       </c>
       <c r="S1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="T1">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="U1">
         <v>90</v>
       </c>
       <c r="V1">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="W1">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="X1">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="Y1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="Z1">
-        <v>315</v>
+        <v>270</v>
       </c>
       <c r="AA1">
-        <v>315</v>
+        <v>225</v>
       </c>
       <c r="AB1">
-        <v>315</v>
+        <v>225</v>
       </c>
       <c r="AC1">
-        <v>315</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.3">
@@ -453,55 +442,55 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="D2">
-        <v>225</v>
+        <v>90</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="F2">
         <v>180</v>
       </c>
       <c r="G2">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="M2">
         <v>180</v>
       </c>
       <c r="N2">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="O2">
-        <v>225</v>
+        <v>315</v>
       </c>
       <c r="P2">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>225</v>
+        <v>90</v>
       </c>
       <c r="R2">
         <v>180</v>
       </c>
       <c r="S2">
-        <v>225</v>
+        <v>90</v>
       </c>
       <c r="T2">
         <v>180</v>
@@ -510,16 +499,16 @@
         <v>180</v>
       </c>
       <c r="V2">
-        <v>225</v>
+        <v>0</v>
       </c>
       <c r="W2">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="X2">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="Y2">
-        <v>225</v>
+        <v>45</v>
       </c>
       <c r="Z2">
         <v>45</v>
@@ -545,7 +534,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E3">
         <v>45</v>
@@ -560,58 +549,58 @@
         <v>45</v>
       </c>
       <c r="I3">
-        <v>180</v>
+        <v>45</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="K3">
         <v>45</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="M3">
         <v>225</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="O3">
-        <v>180</v>
+        <v>225</v>
       </c>
       <c r="P3">
-        <v>180</v>
+        <v>45</v>
       </c>
       <c r="Q3">
-        <v>180</v>
+        <v>225</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>225</v>
       </c>
       <c r="S3">
-        <v>180</v>
+        <v>225</v>
       </c>
       <c r="T3">
-        <v>180</v>
+        <v>225</v>
       </c>
       <c r="U3">
         <v>225</v>
       </c>
       <c r="V3">
-        <v>180</v>
+        <v>45</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="X3">
-        <v>180</v>
+        <v>225</v>
       </c>
       <c r="Y3">
-        <v>180</v>
+        <v>225</v>
       </c>
       <c r="Z3">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="AA3">
         <v>45</v>
@@ -637,61 +626,61 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="F4">
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>315</v>
+        <v>270</v>
       </c>
       <c r="H4">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="I4">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="J4">
-        <v>45</v>
+        <v>180</v>
       </c>
       <c r="K4">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="L4">
-        <v>45</v>
+        <v>180</v>
       </c>
       <c r="M4">
-        <v>315</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>45</v>
+        <v>180</v>
       </c>
       <c r="O4">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>45</v>
+        <v>180</v>
       </c>
       <c r="Q4">
-        <v>225</v>
+        <v>0</v>
       </c>
       <c r="R4">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="S4">
         <v>0</v>
       </c>
       <c r="T4">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="U4">
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="V4">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="W4">
-        <v>45</v>
+        <v>180</v>
       </c>
       <c r="X4">
         <v>0</v>
@@ -700,16 +689,16 @@
         <v>0</v>
       </c>
       <c r="Z4">
-        <v>45</v>
+        <v>180</v>
       </c>
       <c r="AA4">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="AB4">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="AC4">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.3">
@@ -729,76 +718,76 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>270</v>
+        <v>225</v>
       </c>
       <c r="G5">
-        <v>180</v>
+        <v>225</v>
       </c>
       <c r="H5">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="I5">
         <v>45</v>
       </c>
       <c r="J5">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="L5">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="M5">
-        <v>135</v>
+        <v>225</v>
       </c>
       <c r="N5">
-        <v>315</v>
+        <v>45</v>
       </c>
       <c r="O5">
-        <v>270</v>
+        <v>225</v>
       </c>
       <c r="P5">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="Q5">
-        <v>270</v>
+        <v>225</v>
       </c>
       <c r="R5">
-        <v>270</v>
+        <v>225</v>
       </c>
       <c r="S5">
-        <v>135</v>
+        <v>225</v>
       </c>
       <c r="T5">
-        <v>270</v>
+        <v>225</v>
       </c>
       <c r="U5">
-        <v>180</v>
+        <v>225</v>
       </c>
       <c r="V5">
-        <v>90</v>
+        <v>225</v>
       </c>
       <c r="W5">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="X5">
-        <v>270</v>
+        <v>225</v>
       </c>
       <c r="Y5">
-        <v>135</v>
+        <v>45</v>
       </c>
       <c r="Z5">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="AA5">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="AB5">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="AC5">
-        <v>90</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.3">
@@ -821,73 +810,73 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="H6">
-        <v>180</v>
+        <v>315</v>
       </c>
       <c r="I6">
-        <v>90</v>
+        <v>225</v>
       </c>
       <c r="J6">
-        <v>90</v>
+        <v>225</v>
       </c>
       <c r="K6">
-        <v>180</v>
+        <v>315</v>
       </c>
       <c r="L6">
-        <v>90</v>
+        <v>225</v>
       </c>
       <c r="M6">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="N6">
         <v>90</v>
       </c>
       <c r="O6">
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="P6">
-        <v>225</v>
+        <v>315</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="R6">
         <v>135</v>
       </c>
       <c r="S6">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="T6">
-        <v>270</v>
+        <v>135</v>
       </c>
       <c r="U6">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="V6">
-        <v>270</v>
+        <v>135</v>
       </c>
       <c r="W6">
-        <v>225</v>
+        <v>315</v>
       </c>
       <c r="X6">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="Y6">
-        <v>270</v>
+        <v>45</v>
       </c>
       <c r="Z6">
-        <v>225</v>
+        <v>315</v>
       </c>
       <c r="AA6">
-        <v>180</v>
+        <v>315</v>
       </c>
       <c r="AB6">
-        <v>180</v>
+        <v>315</v>
       </c>
       <c r="AC6">
-        <v>180</v>
+        <v>315</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.3">
@@ -913,34 +902,34 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>225</v>
+        <v>315</v>
       </c>
       <c r="I7">
         <v>315</v>
       </c>
       <c r="J7">
-        <v>225</v>
+        <v>90</v>
       </c>
       <c r="K7">
-        <v>180</v>
+        <v>315</v>
       </c>
       <c r="L7">
-        <v>225</v>
+        <v>315</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="N7">
-        <v>225</v>
+        <v>315</v>
       </c>
       <c r="O7">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="P7">
-        <v>225</v>
+        <v>315</v>
       </c>
       <c r="Q7">
-        <v>45</v>
+        <v>270</v>
       </c>
       <c r="R7">
         <v>135</v>
@@ -949,34 +938,34 @@
         <v>135</v>
       </c>
       <c r="T7">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="U7">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="V7">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="W7">
-        <v>225</v>
+        <v>315</v>
       </c>
       <c r="X7">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="Y7">
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="Z7">
-        <v>225</v>
+        <v>315</v>
       </c>
       <c r="AA7">
-        <v>225</v>
+        <v>90</v>
       </c>
       <c r="AB7">
-        <v>180</v>
+        <v>315</v>
       </c>
       <c r="AC7">
-        <v>225</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.3">
@@ -1005,46 +994,46 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="J8">
-        <v>225</v>
+        <v>315</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="M8">
-        <v>180</v>
+        <v>45</v>
       </c>
       <c r="N8">
-        <v>225</v>
+        <v>315</v>
       </c>
       <c r="O8">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="P8">
         <v>225</v>
       </c>
       <c r="Q8">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="R8">
         <v>45</v>
       </c>
       <c r="S8">
-        <v>45</v>
+        <v>225</v>
       </c>
       <c r="T8">
-        <v>45</v>
+        <v>180</v>
       </c>
       <c r="U8">
-        <v>180</v>
+        <v>45</v>
       </c>
       <c r="V8">
-        <v>225</v>
+        <v>45</v>
       </c>
       <c r="W8">
         <v>225</v>
@@ -1053,10 +1042,10 @@
         <v>45</v>
       </c>
       <c r="Y8">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="Z8">
-        <v>225</v>
+        <v>0</v>
       </c>
       <c r="AA8">
         <v>0</v>
@@ -1097,64 +1086,64 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>270</v>
+        <v>45</v>
       </c>
       <c r="K9">
         <v>315</v>
       </c>
       <c r="L9">
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="M9">
-        <v>135</v>
+        <v>45</v>
       </c>
       <c r="N9">
         <v>270</v>
       </c>
       <c r="O9">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="P9">
-        <v>270</v>
+        <v>315</v>
       </c>
       <c r="Q9">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="R9">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="S9">
-        <v>180</v>
+        <v>45</v>
       </c>
       <c r="T9">
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="U9">
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="V9">
         <v>270</v>
       </c>
       <c r="W9">
-        <v>270</v>
+        <v>315</v>
       </c>
       <c r="X9">
-        <v>270</v>
+        <v>225</v>
       </c>
       <c r="Y9">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="Z9">
-        <v>315</v>
+        <v>225</v>
       </c>
       <c r="AA9">
         <v>315</v>
       </c>
       <c r="AB9">
-        <v>315</v>
+        <v>45</v>
       </c>
       <c r="AC9">
-        <v>270</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.3">
@@ -1189,7 +1178,7 @@
         <v>0</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -1210,28 +1199,28 @@
         <v>180</v>
       </c>
       <c r="R10">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="S10">
         <v>180</v>
       </c>
       <c r="T10">
-        <v>180</v>
+        <v>315</v>
       </c>
       <c r="U10">
-        <v>180</v>
+        <v>315</v>
       </c>
       <c r="V10">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="W10">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="X10">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="Y10">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="Z10">
         <v>0</v>
@@ -1240,7 +1229,7 @@
         <v>0</v>
       </c>
       <c r="AB10">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="AC10">
         <v>0</v>
@@ -1281,16 +1270,16 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="M11">
-        <v>315</v>
+        <v>270</v>
       </c>
       <c r="N11">
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="O11">
-        <v>315</v>
+        <v>270</v>
       </c>
       <c r="P11">
         <v>135</v>
@@ -1299,13 +1288,13 @@
         <v>315</v>
       </c>
       <c r="R11">
-        <v>315</v>
+        <v>0</v>
       </c>
       <c r="S11">
-        <v>315</v>
+        <v>225</v>
       </c>
       <c r="T11">
-        <v>315</v>
+        <v>180</v>
       </c>
       <c r="U11">
         <v>180</v>
@@ -1320,13 +1309,13 @@
         <v>315</v>
       </c>
       <c r="Y11">
-        <v>315</v>
+        <v>135</v>
       </c>
       <c r="Z11">
-        <v>135</v>
+        <v>0</v>
       </c>
       <c r="AA11">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="AB11">
         <v>135</v>
@@ -1373,7 +1362,7 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <v>225</v>
+        <v>135</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -1382,22 +1371,22 @@
         <v>180</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="Q12">
-        <v>180</v>
+        <v>135</v>
       </c>
       <c r="R12">
-        <v>180</v>
+        <v>135</v>
       </c>
       <c r="S12">
         <v>180</v>
       </c>
       <c r="T12">
-        <v>180</v>
+        <v>135</v>
       </c>
       <c r="U12">
-        <v>225</v>
+        <v>135</v>
       </c>
       <c r="V12">
         <v>180</v>
@@ -1406,13 +1395,13 @@
         <v>0</v>
       </c>
       <c r="X12">
-        <v>180</v>
+        <v>135</v>
       </c>
       <c r="Y12">
         <v>180</v>
       </c>
       <c r="Z12">
-        <v>0</v>
+        <v>315</v>
       </c>
       <c r="AA12">
         <v>315</v>
@@ -1421,7 +1410,7 @@
         <v>315</v>
       </c>
       <c r="AC12">
-        <v>315</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.3">
@@ -1468,46 +1457,46 @@
         <v>90</v>
       </c>
       <c r="O13">
-        <v>270</v>
+        <v>90</v>
       </c>
       <c r="P13">
-        <v>90</v>
+        <v>270</v>
       </c>
       <c r="Q13">
-        <v>315</v>
+        <v>0</v>
       </c>
       <c r="R13">
-        <v>270</v>
+        <v>315</v>
       </c>
       <c r="S13">
-        <v>270</v>
+        <v>90</v>
       </c>
       <c r="T13">
         <v>315</v>
       </c>
       <c r="U13">
-        <v>0</v>
+        <v>315</v>
       </c>
       <c r="V13">
-        <v>270</v>
+        <v>135</v>
       </c>
       <c r="W13">
-        <v>90</v>
+        <v>270</v>
       </c>
       <c r="X13">
-        <v>270</v>
+        <v>315</v>
       </c>
       <c r="Y13">
-        <v>270</v>
+        <v>90</v>
       </c>
       <c r="Z13">
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="AA13">
         <v>135</v>
       </c>
       <c r="AB13">
-        <v>180</v>
+        <v>135</v>
       </c>
       <c r="AC13">
         <v>135</v>
@@ -1560,43 +1549,43 @@
         <v>135</v>
       </c>
       <c r="P14">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="Q14">
         <v>180</v>
       </c>
       <c r="R14">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="S14">
-        <v>135</v>
+        <v>315</v>
       </c>
       <c r="T14">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="U14">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="V14">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="W14">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="X14">
         <v>270</v>
       </c>
       <c r="Y14">
-        <v>315</v>
+        <v>180</v>
       </c>
       <c r="Z14">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="AA14">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="AB14">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="AC14">
         <v>90</v>
@@ -1649,34 +1638,34 @@
         <v>0</v>
       </c>
       <c r="P15">
-        <v>315</v>
+        <v>45</v>
       </c>
       <c r="Q15">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="R15">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="S15">
-        <v>0</v>
+        <v>225</v>
       </c>
       <c r="T15">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="U15">
         <v>45</v>
       </c>
       <c r="V15">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="W15">
-        <v>315</v>
+        <v>45</v>
       </c>
       <c r="X15">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="Y15">
-        <v>315</v>
+        <v>180</v>
       </c>
       <c r="Z15">
         <v>225</v>
@@ -1685,10 +1674,10 @@
         <v>225</v>
       </c>
       <c r="AB15">
-        <v>225</v>
+        <v>315</v>
       </c>
       <c r="AC15">
-        <v>225</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.3">
@@ -1747,37 +1736,37 @@
         <v>135</v>
       </c>
       <c r="S16">
-        <v>270</v>
+        <v>135</v>
       </c>
       <c r="T16">
-        <v>225</v>
+        <v>135</v>
       </c>
       <c r="U16">
         <v>180</v>
       </c>
       <c r="V16">
-        <v>315</v>
+        <v>180</v>
       </c>
       <c r="W16">
-        <v>0</v>
+        <v>315</v>
       </c>
       <c r="X16">
         <v>135</v>
       </c>
       <c r="Y16">
-        <v>315</v>
+        <v>135</v>
       </c>
       <c r="Z16">
         <v>315</v>
       </c>
       <c r="AA16">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="AB16">
-        <v>315</v>
+        <v>45</v>
       </c>
       <c r="AC16">
-        <v>45</v>
+        <v>315</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.3">
@@ -1836,7 +1825,7 @@
         <v>0</v>
       </c>
       <c r="S17">
-        <v>225</v>
+        <v>0</v>
       </c>
       <c r="T17">
         <v>0</v>
@@ -1845,16 +1834,16 @@
         <v>0</v>
       </c>
       <c r="V17">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="W17">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="X17">
-        <v>225</v>
+        <v>0</v>
       </c>
       <c r="Y17">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="Z17">
         <v>180</v>
@@ -1928,34 +1917,34 @@
         <v>180</v>
       </c>
       <c r="T18">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="U18">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="V18">
-        <v>0</v>
+        <v>315</v>
       </c>
       <c r="W18">
         <v>270</v>
       </c>
       <c r="X18">
-        <v>180</v>
+        <v>315</v>
       </c>
       <c r="Y18">
-        <v>90</v>
+        <v>270</v>
       </c>
       <c r="Z18">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="AA18">
         <v>270</v>
       </c>
       <c r="AB18">
-        <v>225</v>
+        <v>315</v>
       </c>
       <c r="AC18">
-        <v>180</v>
+        <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.3">
@@ -2017,25 +2006,25 @@
         <v>0</v>
       </c>
       <c r="T19">
-        <v>0</v>
+        <v>315</v>
       </c>
       <c r="U19">
         <v>315</v>
       </c>
       <c r="V19">
-        <v>225</v>
+        <v>315</v>
       </c>
       <c r="W19">
-        <v>225</v>
+        <v>45</v>
       </c>
       <c r="X19">
-        <v>45</v>
+        <v>315</v>
       </c>
       <c r="Y19">
-        <v>225</v>
+        <v>315</v>
       </c>
       <c r="Z19">
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="AA19">
         <v>135</v>
@@ -2112,28 +2101,28 @@
         <v>0</v>
       </c>
       <c r="V20">
-        <v>0</v>
+        <v>225</v>
       </c>
       <c r="W20">
-        <v>180</v>
+        <v>135</v>
       </c>
       <c r="X20">
-        <v>0</v>
+        <v>315</v>
       </c>
       <c r="Y20">
         <v>135</v>
       </c>
       <c r="Z20">
-        <v>180</v>
+        <v>135</v>
       </c>
       <c r="AA20">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="AB20">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="AC20">
-        <v>180</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.3">
@@ -2201,28 +2190,28 @@
         <v>0</v>
       </c>
       <c r="V21">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="W21">
-        <v>135</v>
+        <v>315</v>
       </c>
       <c r="X21">
         <v>315</v>
       </c>
       <c r="Y21">
-        <v>135</v>
+        <v>315</v>
       </c>
       <c r="Z21">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="AA21">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="AB21">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="AC21">
-        <v>270</v>
+        <v>315</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.3">
@@ -2293,25 +2282,25 @@
         <v>0</v>
       </c>
       <c r="W22">
-        <v>0</v>
+        <v>315</v>
       </c>
       <c r="X22">
-        <v>180</v>
+        <v>315</v>
       </c>
       <c r="Y22">
-        <v>180</v>
+        <v>315</v>
       </c>
       <c r="Z22">
-        <v>315</v>
+        <v>225</v>
       </c>
       <c r="AA22">
-        <v>270</v>
+        <v>315</v>
       </c>
       <c r="AB22">
         <v>270</v>
       </c>
       <c r="AC22">
-        <v>225</v>
+        <v>315</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.3">
@@ -2385,22 +2374,22 @@
         <v>0</v>
       </c>
       <c r="X23">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="Y23">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="Z23">
         <v>0</v>
       </c>
       <c r="AA23">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="AB23">
-        <v>315</v>
+        <v>45</v>
       </c>
       <c r="AC23">
-        <v>45</v>
+        <v>315</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
@@ -2480,13 +2469,13 @@
         <v>0</v>
       </c>
       <c r="Z24">
-        <v>225</v>
+        <v>45</v>
       </c>
       <c r="AA24">
         <v>225</v>
       </c>
       <c r="AB24">
-        <v>225</v>
+        <v>315</v>
       </c>
       <c r="AC24">
         <v>225</v>
@@ -2572,10 +2561,10 @@
         <v>225</v>
       </c>
       <c r="AA25">
-        <v>315</v>
+        <v>225</v>
       </c>
       <c r="AB25">
-        <v>315</v>
+        <v>90</v>
       </c>
       <c r="AC25">
         <v>225</v>
@@ -2661,13 +2650,13 @@
         <v>0</v>
       </c>
       <c r="AA26">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="AB26">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="AC26">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.3">
@@ -2756,7 +2745,7 @@
         <v>0</v>
       </c>
       <c r="AC27">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.3">
@@ -2845,7 +2834,7 @@
         <v>0</v>
       </c>
       <c r="AC28">
-        <v>315</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.3">
@@ -2939,6 +2928,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>